<commit_message>
First implementation of readBEAMsim
</commit_message>
<xml_diff>
--- a/11-Parameters/LhARABeamLine-Params-LsrDrvn-Gabor.xlsx
+++ b/11-Parameters/LhARABeamLine-Params-LsrDrvn-Gabor.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ken.long/KL-GIT/CCAP/02-LhARA/04-LhARAlinearOptics/11-Parameters/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kennethlong/KL-GIT/CCAP/02-LhARA/04-LhARAlinearOptics/11-Parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{95AC6016-9443-C246-89B9-5AA81BEA8D57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66C9300D-B692-234F-A5FB-E49E5E00B1BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6040" yWindow="640" windowWidth="21660" windowHeight="19000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21800" yWindow="6800" windowWidth="21660" windowHeight="19000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LhARABeamLine-Params-LsrDrvn" sheetId="1" r:id="rId1"/>
@@ -68,9 +68,6 @@
     <t>SourceMode</t>
   </si>
   <si>
-    <t>Gaussian kinetic energy</t>
-  </si>
-  <si>
     <t>MeV</t>
   </si>
   <si>
@@ -345,6 +342,9 @@
   </si>
   <si>
     <t>Drift to next Gabor lens</t>
+  </si>
+  <si>
+    <t>Mode</t>
   </si>
 </sst>
 </file>
@@ -544,9 +544,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -584,7 +584,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -690,7 +690,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -832,7 +832,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -843,7 +843,7 @@
   <dimension ref="A1:H99"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -869,7 +869,7 @@
         <v>7</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>0</v>
@@ -889,11 +889,11 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="D2" s="1" t="s">
         <v>1</v>
       </c>
@@ -901,7 +901,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
@@ -911,22 +911,22 @@
         <v>0</v>
       </c>
       <c r="B3" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="D3" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="E3" s="8" t="s">
         <v>33</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>34</v>
       </c>
       <c r="F3" s="8">
         <v>15</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H3" s="8"/>
     </row>
@@ -935,22 +935,22 @@
         <v>0</v>
       </c>
       <c r="B4" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>32</v>
-      </c>
       <c r="D4" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="E4" s="9" t="s">
         <v>60</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>61</v>
       </c>
       <c r="F4" s="9">
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H4" s="9"/>
     </row>
@@ -965,7 +965,7 @@
         <v>8</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E5" s="10" t="s">
         <v>9</v>
@@ -975,7 +975,7 @@
       </c>
       <c r="G5" s="10"/>
       <c r="H5" s="10" t="s">
-        <v>10</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -989,19 +989,19 @@
         <v>8</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F6" s="11">
         <v>3.9999999999999998E-6</v>
       </c>
       <c r="G6" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="11" t="s">
         <v>14</v>
-      </c>
-      <c r="H6" s="11" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -1015,19 +1015,19 @@
         <v>8</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F7" s="11">
         <v>3.9999999999999998E-6</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -1041,19 +1041,19 @@
         <v>8</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F8" s="11">
         <v>1</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -1067,19 +1067,19 @@
         <v>8</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F9" s="12">
         <v>25</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H9" s="12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -1093,17 +1093,17 @@
         <v>8</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F10" s="5">
         <v>1000</v>
       </c>
       <c r="G10" s="5"/>
       <c r="H10" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -1117,17 +1117,17 @@
         <v>8</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F11" s="5">
         <v>0.99969115500000005</v>
       </c>
       <c r="G11" s="5"/>
       <c r="H11" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -1141,19 +1141,19 @@
         <v>8</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F12" s="5">
         <v>2500000000000000</v>
       </c>
       <c r="G12" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="H12" s="5" t="s">
         <v>76</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -1167,19 +1167,19 @@
         <v>8</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F13" s="5">
         <v>70</v>
       </c>
       <c r="G13" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="H13" s="5" t="s">
         <v>79</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
@@ -1193,19 +1193,19 @@
         <v>8</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F14" s="5">
         <v>0.8</v>
       </c>
       <c r="G14" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="H14" s="5" t="s">
         <v>82</v>
-      </c>
-      <c r="H14" s="5" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
@@ -1219,19 +1219,19 @@
         <v>8</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F15" s="13">
         <v>2.8000000000000001E-14</v>
       </c>
       <c r="G15" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="H15" s="5" t="s">
         <v>85</v>
-      </c>
-      <c r="H15" s="5" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
@@ -1245,19 +1245,19 @@
         <v>8</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F16">
         <v>3.9999999999999998E-7</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
@@ -1271,19 +1271,19 @@
         <v>8</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F17" s="13">
         <v>4E+20</v>
       </c>
       <c r="G17" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H17" s="5" t="s">
         <v>90</v>
-      </c>
-      <c r="H17" s="5" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
@@ -1297,19 +1297,19 @@
         <v>8</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F18" s="3">
         <v>25</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
@@ -1317,23 +1317,23 @@
         <v>1</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D19" s="4"/>
       <c r="E19" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F19" s="4">
         <v>0.05</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
@@ -1341,25 +1341,25 @@
         <v>1</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F20" s="5">
         <v>2E-3</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
@@ -1367,23 +1367,23 @@
         <v>1</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D21" s="5"/>
       <c r="E21" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F21" s="5">
         <v>0.05</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
@@ -1391,25 +1391,25 @@
         <v>1</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F22" s="3">
         <v>2.8700000000000002E-3</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
@@ -1417,23 +1417,23 @@
         <v>1</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D23" s="4"/>
       <c r="E23" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F23" s="4">
         <v>0.15</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
@@ -1441,25 +1441,25 @@
         <v>1</v>
       </c>
       <c r="B24" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="D24" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C24" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>41</v>
-      </c>
       <c r="E24" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F24" s="5">
         <v>0.85699999999999998</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
@@ -1467,26 +1467,26 @@
         <v>1</v>
       </c>
       <c r="B25" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="D25" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C25" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="D25" s="5" t="s">
+      <c r="E25" s="5" t="s">
         <v>41</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>42</v>
       </c>
       <c r="F25" s="5">
         <f>2.4916949087545</f>
         <v>2.4916949087544999</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
@@ -1494,23 +1494,23 @@
         <v>1</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D26" s="5"/>
       <c r="E26" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F26" s="5">
         <v>0.15</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
@@ -1518,23 +1518,23 @@
         <v>1</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D27" s="5"/>
       <c r="E27" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F27" s="5">
         <v>0.15</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
@@ -1542,25 +1542,25 @@
         <v>1</v>
       </c>
       <c r="B28" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="D28" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C28" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>41</v>
-      </c>
       <c r="E28" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F28" s="5">
         <v>0.85699999999999998</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
@@ -1568,25 +1568,25 @@
         <v>1</v>
       </c>
       <c r="B29" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="D29" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C29" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="D29" s="5" t="s">
+      <c r="E29" s="5" t="s">
         <v>41</v>
-      </c>
-      <c r="E29" s="5" t="s">
-        <v>42</v>
       </c>
       <c r="F29" s="5">
         <v>1.0187472612650501</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
@@ -1594,23 +1594,23 @@
         <v>1</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D30" s="3"/>
       <c r="E30" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F30" s="3">
         <v>0.15</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
@@ -1618,24 +1618,24 @@
         <v>1</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D31" s="4"/>
       <c r="E31" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F31" s="4">
         <f>(0.5-0.132433454701889)/2</f>
         <v>0.1837832726490555</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
@@ -1643,25 +1643,25 @@
         <v>1</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C32" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D32" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="D32" s="5" t="s">
+      <c r="E32" s="5" t="s">
         <v>65</v>
-      </c>
-      <c r="E32" s="5" t="s">
-        <v>66</v>
       </c>
       <c r="F32" s="5">
         <v>5</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H32" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
@@ -1669,25 +1669,25 @@
         <v>1</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C33" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D33" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="D33" s="5" t="s">
-        <v>65</v>
-      </c>
       <c r="E33" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F33" s="5">
         <v>200</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
@@ -1695,25 +1695,25 @@
         <v>1</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C34" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D34" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="D34" s="5" t="s">
-        <v>65</v>
-      </c>
       <c r="E34" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F34" s="5">
         <v>0</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H34" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
@@ -1721,24 +1721,24 @@
         <v>1</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D35" s="5"/>
       <c r="E35" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F35" s="5">
         <f>(0.5-0.132433454701889)/2</f>
         <v>0.1837832726490555</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H35" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
@@ -1746,23 +1746,23 @@
         <v>1</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D36" s="5"/>
       <c r="E36" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F36" s="5">
         <v>0.15</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H36" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
@@ -1770,22 +1770,22 @@
         <v>1</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F37" s="5">
         <v>0.85699999999999998</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H37" s="5"/>
     </row>
@@ -1794,22 +1794,22 @@
         <v>1</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D38" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E38" s="5" t="s">
         <v>41</v>
-      </c>
-      <c r="E38" s="5" t="s">
-        <v>42</v>
       </c>
       <c r="F38" s="5">
         <v>1.4485646330252</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H38" s="5"/>
     </row>
@@ -1818,23 +1818,23 @@
         <v>1</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D39" s="5"/>
       <c r="E39" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F39" s="5">
         <v>0.15</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H39" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
@@ -1842,23 +1842,23 @@
         <v>1</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D40" s="5"/>
       <c r="E40" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F40" s="5">
         <v>1.7709999999999999</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H40" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
@@ -1866,23 +1866,23 @@
         <v>1</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D41" s="5"/>
       <c r="E41" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F41" s="5">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H41" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
@@ -1890,25 +1890,25 @@
         <v>1</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F42" s="5">
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H42" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
@@ -1916,23 +1916,23 @@
         <v>1</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D43" s="5"/>
       <c r="E43" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F43" s="5">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H43" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
@@ -1940,20 +1940,20 @@
         <v>1</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D44" s="5"/>
       <c r="E44" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F44" s="5">
         <v>6.4610000000000001E-2</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H44" s="5"/>
     </row>
@@ -1962,20 +1962,20 @@
         <v>1</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D45" s="5"/>
       <c r="E45" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F45" s="5">
         <v>0.13539000000000001</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H45" s="5"/>
     </row>
@@ -1984,23 +1984,23 @@
         <v>1</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D46" s="5"/>
       <c r="E46" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F46" s="5">
         <v>0.01</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H46" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
@@ -2008,20 +2008,20 @@
         <v>1</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D47" s="5"/>
       <c r="E47" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F47" s="5">
         <v>5.4600000000000003E-2</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H47" s="5"/>
     </row>
@@ -2030,24 +2030,24 @@
         <v>1</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D48" s="5"/>
       <c r="E48" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F48" s="5">
         <f>(0.5-0.132433454701889)/2</f>
         <v>0.1837832726490555</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H48" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
@@ -2055,25 +2055,25 @@
         <v>1</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C49" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D49" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="D49" s="5" t="s">
+      <c r="E49" s="5" t="s">
         <v>65</v>
-      </c>
-      <c r="E49" s="5" t="s">
-        <v>66</v>
       </c>
       <c r="F49" s="5">
         <v>5</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H49" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
@@ -2081,25 +2081,25 @@
         <v>1</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C50" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D50" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="D50" s="5" t="s">
-        <v>65</v>
-      </c>
       <c r="E50" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F50" s="5">
         <v>200</v>
       </c>
       <c r="G50" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H50" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
@@ -2107,25 +2107,25 @@
         <v>1</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C51" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D51" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="D51" s="5" t="s">
-        <v>65</v>
-      </c>
       <c r="E51" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F51" s="5">
         <v>0</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H51" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
@@ -2133,24 +2133,24 @@
         <v>1</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D52" s="5"/>
       <c r="E52" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F52" s="5">
         <f>(0.5-0.132433454701889)/2</f>
         <v>0.1837832726490555</v>
       </c>
       <c r="G52" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H52" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
@@ -2158,23 +2158,23 @@
         <v>1</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D53" s="4"/>
       <c r="E53" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F53" s="4">
         <v>0.15</v>
       </c>
       <c r="G53" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H53" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
@@ -2182,22 +2182,22 @@
         <v>1</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F54" s="5">
         <v>0.85699999999999998</v>
       </c>
       <c r="G54" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H54" s="5"/>
     </row>
@@ -2206,22 +2206,22 @@
         <v>1</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D55" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E55" s="5" t="s">
         <v>41</v>
-      </c>
-      <c r="E55" s="5" t="s">
-        <v>42</v>
       </c>
       <c r="F55" s="5">
         <v>1.7888589662779599</v>
       </c>
       <c r="G55" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H55" s="5"/>
     </row>
@@ -2230,23 +2230,23 @@
         <v>1</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D56" s="5"/>
       <c r="E56" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F56" s="5">
         <v>0.15</v>
       </c>
       <c r="G56" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H56" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
@@ -2254,20 +2254,20 @@
         <v>1</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D57" s="5"/>
       <c r="E57" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F57" s="5">
         <v>0.3</v>
       </c>
       <c r="G57" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H57" s="5"/>
     </row>
@@ -2276,23 +2276,23 @@
         <v>1</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D58" s="5"/>
       <c r="E58" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F58" s="5">
         <v>0.15</v>
       </c>
       <c r="G58" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H58" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
@@ -2300,22 +2300,22 @@
         <v>1</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E59" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F59" s="5">
         <v>0.85699999999999998</v>
       </c>
       <c r="G59" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H59" s="5"/>
     </row>
@@ -2324,22 +2324,22 @@
         <v>1</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D60" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E60" s="5" t="s">
         <v>41</v>
-      </c>
-      <c r="E60" s="5" t="s">
-        <v>42</v>
       </c>
       <c r="F60" s="5">
         <v>1.60433994066042</v>
       </c>
       <c r="G60" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H60" s="5"/>
     </row>
@@ -2348,23 +2348,23 @@
         <v>1</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D61" s="5"/>
       <c r="E61" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F61" s="5">
         <v>0.15</v>
       </c>
       <c r="G61" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H61" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
@@ -2372,20 +2372,20 @@
         <v>1</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D62" s="5"/>
       <c r="E62" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F62" s="5">
         <v>2.5</v>
       </c>
       <c r="G62" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H62" s="5"/>
     </row>
@@ -2394,23 +2394,23 @@
         <v>1</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D63" s="5"/>
       <c r="E63" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F63" s="5">
         <v>0.15</v>
       </c>
       <c r="G63" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H63" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
@@ -2418,22 +2418,22 @@
         <v>1</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E64" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F64" s="5">
         <v>0.85699999999999998</v>
       </c>
       <c r="G64" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H64" s="5"/>
     </row>
@@ -2442,22 +2442,22 @@
         <v>1</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D65" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E65" s="5" t="s">
         <v>41</v>
-      </c>
-      <c r="E65" s="5" t="s">
-        <v>42</v>
       </c>
       <c r="F65" s="5">
         <v>1.2448140165275099</v>
       </c>
       <c r="G65" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H65" s="5"/>
     </row>
@@ -2466,23 +2466,23 @@
         <v>1</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D66" s="5"/>
       <c r="E66" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F66" s="5">
         <v>0.15</v>
       </c>
       <c r="G66" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H66" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
@@ -2490,20 +2490,20 @@
         <v>1</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D67" s="5"/>
       <c r="E67" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F67" s="5">
         <v>0.3</v>
       </c>
       <c r="G67" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H67" s="5"/>
     </row>
@@ -2512,23 +2512,23 @@
         <v>1</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D68" s="5"/>
       <c r="E68" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F68" s="5">
         <v>0.15</v>
       </c>
       <c r="G68" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H68" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.2">
@@ -2536,22 +2536,22 @@
         <v>1</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D69" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E69" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F69" s="5">
         <v>0.85699999999999998</v>
       </c>
       <c r="G69" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H69" s="5"/>
     </row>
@@ -2560,22 +2560,22 @@
         <v>1</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D70" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E70" s="5" t="s">
         <v>41</v>
-      </c>
-      <c r="E70" s="5" t="s">
-        <v>42</v>
       </c>
       <c r="F70" s="5">
         <v>1.1659674896013299</v>
       </c>
       <c r="G70" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H70" s="5"/>
     </row>
@@ -2584,23 +2584,23 @@
         <v>1</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D71" s="3"/>
       <c r="E71" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F71" s="3">
         <v>0.15</v>
       </c>
       <c r="G71" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H71" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
@@ -2608,20 +2608,20 @@
         <v>1</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C72" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D72" s="5"/>
       <c r="E72" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F72" s="5">
         <v>0.2</v>
       </c>
       <c r="G72" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H72" s="5"/>
     </row>
@@ -2630,22 +2630,22 @@
         <v>1</v>
       </c>
       <c r="B73" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C73" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C73" s="5" t="s">
-        <v>52</v>
-      </c>
       <c r="D73" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E73" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F73" s="5">
         <v>0.8</v>
       </c>
       <c r="G73" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H73" s="5"/>
     </row>
@@ -2654,22 +2654,22 @@
         <v>1</v>
       </c>
       <c r="B74" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C74" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C74" s="5" t="s">
+      <c r="D74" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E74" s="5" t="s">
         <v>52</v>
-      </c>
-      <c r="D74" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="E74" s="5" t="s">
-        <v>53</v>
       </c>
       <c r="F74" s="5">
         <v>45</v>
       </c>
       <c r="G74" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H74" s="5"/>
     </row>
@@ -2678,20 +2678,20 @@
         <v>1</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C75" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D75" s="5"/>
       <c r="E75" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F75" s="5">
         <v>0.2</v>
       </c>
       <c r="G75" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H75" s="5"/>
     </row>
@@ -2700,20 +2700,20 @@
         <v>1</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C76" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D76" s="5"/>
       <c r="E76" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F76" s="5">
         <v>0.1</v>
       </c>
       <c r="G76" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H76" s="5"/>
     </row>
@@ -2722,20 +2722,20 @@
         <v>1</v>
       </c>
       <c r="B77" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C77" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D77" s="5"/>
       <c r="E77" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F77" s="5">
         <v>22.544</v>
       </c>
       <c r="G77" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H77" s="5"/>
     </row>
@@ -2744,20 +2744,20 @@
         <v>1</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C78" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D78" s="5"/>
       <c r="E78" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F78" s="5">
         <v>0.4</v>
       </c>
       <c r="G78" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H78" s="5"/>
     </row>
@@ -2766,20 +2766,20 @@
         <v>1</v>
       </c>
       <c r="B79" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C79" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D79" s="5"/>
       <c r="E79" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F79" s="5">
         <v>0.1</v>
       </c>
       <c r="G79" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H79" s="5"/>
     </row>
@@ -2788,20 +2788,20 @@
         <v>1</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C80" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D80" s="5"/>
       <c r="E80" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F80" s="5">
         <v>31.376799999999999</v>
       </c>
       <c r="G80" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H80" s="5"/>
     </row>
@@ -2810,20 +2810,20 @@
         <v>1</v>
       </c>
       <c r="B81" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C81" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D81" s="5"/>
       <c r="E81" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F81" s="5">
         <v>0.2</v>
       </c>
       <c r="G81" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H81" s="5"/>
     </row>
@@ -2832,20 +2832,20 @@
         <v>1</v>
       </c>
       <c r="B82" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C82" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D82" s="5"/>
       <c r="E82" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F82" s="5">
         <v>0.1</v>
       </c>
       <c r="G82" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H82" s="5"/>
     </row>
@@ -2854,20 +2854,20 @@
         <v>1</v>
       </c>
       <c r="B83" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C83" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D83" s="5"/>
       <c r="E83" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F83" s="5">
         <v>31.5123</v>
       </c>
       <c r="G83" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H83" s="5"/>
     </row>
@@ -2876,21 +2876,21 @@
         <v>1</v>
       </c>
       <c r="B84" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C84" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D84" s="5"/>
       <c r="E84" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F84" s="5">
         <f>0.2-0.005</f>
         <v>0.19500000000000001</v>
       </c>
       <c r="G84" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H84" s="5"/>
     </row>
@@ -2899,20 +2899,20 @@
         <v>1</v>
       </c>
       <c r="B85" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C85" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D85" s="5"/>
       <c r="E85" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F85" s="5">
         <v>0.01</v>
       </c>
       <c r="G85" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H85" s="5"/>
     </row>
@@ -2921,21 +2921,21 @@
         <v>1</v>
       </c>
       <c r="B86" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C86" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D86" s="5"/>
       <c r="E86" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F86" s="5">
         <f>0.2-0.005</f>
         <v>0.19500000000000001</v>
       </c>
       <c r="G86" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H86" s="5"/>
     </row>
@@ -2944,20 +2944,20 @@
         <v>1</v>
       </c>
       <c r="B87" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C87" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D87" s="5"/>
       <c r="E87" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F87" s="5">
         <v>0.1</v>
       </c>
       <c r="G87" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H87" s="5"/>
     </row>
@@ -2966,21 +2966,21 @@
         <v>1</v>
       </c>
       <c r="B88" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C88" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D88" s="5"/>
       <c r="E88" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F88" s="5">
         <f>F83</f>
         <v>31.5123</v>
       </c>
       <c r="G88" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H88" s="5"/>
     </row>
@@ -2989,20 +2989,20 @@
         <v>1</v>
       </c>
       <c r="B89" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C89" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D89" s="5"/>
       <c r="E89" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F89" s="5">
         <v>0.2</v>
       </c>
       <c r="G89" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H89" s="5"/>
     </row>
@@ -3011,20 +3011,20 @@
         <v>1</v>
       </c>
       <c r="B90" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C90" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D90" s="5"/>
       <c r="E90" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F90" s="5">
         <v>0.1</v>
       </c>
       <c r="G90" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H90" s="5"/>
     </row>
@@ -3033,21 +3033,21 @@
         <v>1</v>
       </c>
       <c r="B91" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C91" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D91" s="5"/>
       <c r="E91" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F91" s="5">
         <f>F80</f>
         <v>31.376799999999999</v>
       </c>
       <c r="G91" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H91" s="5"/>
     </row>
@@ -3056,20 +3056,20 @@
         <v>1</v>
       </c>
       <c r="B92" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C92" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D92" s="5"/>
       <c r="E92" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F92" s="5">
         <v>0.4</v>
       </c>
       <c r="G92" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H92" s="5"/>
     </row>
@@ -3078,20 +3078,20 @@
         <v>1</v>
       </c>
       <c r="B93" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C93" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D93" s="5"/>
       <c r="E93" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F93" s="5">
         <v>0.1</v>
       </c>
       <c r="G93" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H93" s="5"/>
     </row>
@@ -3100,21 +3100,21 @@
         <v>1</v>
       </c>
       <c r="B94" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C94" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D94" s="5"/>
       <c r="E94" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F94" s="5">
         <f>F77</f>
         <v>22.544</v>
       </c>
       <c r="G94" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H94" s="5"/>
     </row>
@@ -3123,20 +3123,20 @@
         <v>1</v>
       </c>
       <c r="B95" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C95" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D95" s="5"/>
       <c r="E95" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F95" s="5">
         <v>0.2</v>
       </c>
       <c r="G95" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H95" s="5"/>
     </row>
@@ -3145,22 +3145,22 @@
         <v>1</v>
       </c>
       <c r="B96" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C96" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C96" s="5" t="s">
-        <v>52</v>
-      </c>
       <c r="D96" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E96" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F96" s="5">
         <v>0.8</v>
       </c>
       <c r="G96" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H96" s="5"/>
     </row>
@@ -3169,22 +3169,22 @@
         <v>1</v>
       </c>
       <c r="B97" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C97" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C97" s="5" t="s">
+      <c r="D97" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E97" s="5" t="s">
         <v>52</v>
-      </c>
-      <c r="D97" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="E97" s="5" t="s">
-        <v>53</v>
       </c>
       <c r="F97" s="5">
         <v>45</v>
       </c>
       <c r="G97" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H97" s="5"/>
     </row>
@@ -3193,20 +3193,20 @@
         <v>1</v>
       </c>
       <c r="B98" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C98" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D98" s="5"/>
       <c r="E98" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F98" s="5">
         <v>0.2</v>
       </c>
       <c r="G98" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H98" s="5"/>
     </row>
@@ -3215,20 +3215,20 @@
         <v>1</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D99" s="3"/>
       <c r="E99" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F99" s="3">
         <v>2</v>
       </c>
       <c r="G99" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H99" s="3"/>
     </row>

</xml_diff>

<commit_message>
Issues at low energy, worked around in particle
</commit_message>
<xml_diff>
--- a/11-Parameters/LhARABeamLine-Params-LsrDrvn-Gabor.xlsx
+++ b/11-Parameters/LhARABeamLine-Params-LsrDrvn-Gabor.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kennethlong/KL-GIT/CCAP/02-LhARA/04-LhARAlinearOptics/11-Parameters/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/longkr/KL-GIT/CCAP/02-LhARA/04-LhARAlinearOptics/11-Parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F085AB3-F1C8-A24C-91F4-1677D6F3A000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{5E196450-7188-7C4D-821E-8C8FBCF41104}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35940" yWindow="0" windowWidth="21660" windowHeight="32400" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38400" yWindow="0" windowWidth="21660" windowHeight="21600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="LhARABeamLine-Params-LsrDrvn" sheetId="1" r:id="rId1"/>
+    <sheet name="LhARABeamLine-Params-LsrDrvn-Ga" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -861,8 +861,8 @@
   <dimension ref="A1:H103"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>